<commit_message>
update column name to nodeid_linkid
</commit_message>
<xml_diff>
--- a/create_sensor_fault_scenarios.xlsx
+++ b/create_sensor_fault_scenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucy-my.sharepoint.com/personal/mkiria01_ucy_ac_cy/Documents/GITHUB/WDN-Dataset-Generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{177B29A7-7879-400D-9CC1-CDB37F6E079D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{7700E2FD-8218-44B6-9329-EB024F18C5C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{F894360A-DD72-4ABA-A24A-C3E0C20D13F7}"/>
   </bookViews>
@@ -36,9 +36,6 @@
     <t>profile</t>
   </si>
   <si>
-    <t>nodeid/linkid</t>
-  </si>
-  <si>
     <t>sensortype</t>
   </si>
   <si>
@@ -64,6 +61,9 @@
   </si>
   <si>
     <t>normal</t>
+  </si>
+  <si>
+    <t>nodeid_linkid</t>
   </si>
 </sst>
 </file>
@@ -421,7 +421,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,16 +439,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
       <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
         <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -465,7 +465,7 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1">
         <v>43108.5625</v>
@@ -474,7 +474,7 @@
         <v>43131.996527777781</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G2">
         <v>3</v>
@@ -488,7 +488,7 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1">
         <v>43108.5625</v>
@@ -497,7 +497,7 @@
         <v>43131.996527777781</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -511,7 +511,7 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1">
         <v>43108.5625</v>
@@ -520,7 +520,7 @@
         <v>43131.996527777781</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G4">
         <v>2</v>
@@ -533,6 +533,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D653371BCFF1A548A9528A66D553DF4D" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4b0292876563dd01334f32600faea9d5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8629473f-95fa-4c6e-b357-195ffae93069" xmlns:ns4="295eb239-bd93-4f68-a376-d5791a2db291" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a57372c49d8016c83ddf057ea351e794" ns3:_="" ns4:_="">
     <xsd:import namespace="8629473f-95fa-4c6e-b357-195ffae93069"/>
@@ -761,22 +776,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9EFE31D4-504C-4D90-9A60-50CB7265A2C2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="295eb239-bd93-4f68-a376-d5791a2db291"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="8629473f-95fa-4c6e-b357-195ffae93069"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{601637A7-0187-4F30-B4EA-344CFC765FE8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{883DECAC-DC86-4605-B822-B32F2987BEAB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -793,29 +818,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{601637A7-0187-4F30-B4EA-344CFC765FE8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9EFE31D4-504C-4D90-9A60-50CB7265A2C2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="295eb239-bd93-4f68-a376-d5791a2db291"/>
-    <ds:schemaRef ds:uri="8629473f-95fa-4c6e-b357-195ffae93069"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>